<commit_message>
Small changes to test files and documentation
</commit_message>
<xml_diff>
--- a/TimingResults.xlsx
+++ b/TimingResults.xlsx
@@ -2,20 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sophie\Documents\UCL\Disco\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Wallet" sheetId="1" r:id="rId1"/>
     <sheet name="Merchant" sheetId="2" r:id="rId2"/>
     <sheet name="Bank" sheetId="3" r:id="rId3"/>
     <sheet name="All" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="24">
   <si>
     <t>blshim.spending_2</t>
   </si>
@@ -90,6 +92,15 @@
   </si>
   <si>
     <t>blshim.rev_attribute_2</t>
+  </si>
+  <si>
+    <t>bn</t>
+  </si>
+  <si>
+    <t>python</t>
+  </si>
+  <si>
+    <t>self</t>
   </si>
 </sst>
 </file>
@@ -160,6 +171,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Method Timings</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -193,13 +229,28 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
@@ -215,10 +266,11 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -230,10 +282,11 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -245,12 +298,11 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -262,12 +314,11 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -279,12 +330,11 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -296,13 +346,11 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -314,13 +362,11 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -332,13 +378,11 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -350,12 +394,11 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="80000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -367,12 +410,11 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="80000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -384,12 +426,11 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="80000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -401,13 +442,11 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -419,13 +458,11 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -437,13 +474,11 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="14"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -455,12 +490,11 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="15"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -472,12 +506,11 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="16"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -614,10 +647,230 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+        <c:gapWidth val="100"/>
+        <c:axId val="378283704"/>
+        <c:axId val="378277040"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="378283704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Method name</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="378277040"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="378277040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time taken (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="378283704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -626,38 +879,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -710,6 +931,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Web Service Timings</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -743,13 +989,28 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
@@ -765,10 +1026,11 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -780,10 +1042,11 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -795,10 +1058,11 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -857,10 +1121,235 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+        <c:gapWidth val="100"/>
+        <c:axId val="378277824"/>
+        <c:axId val="378283312"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="378277824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Web</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> service name</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="378283312"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="378283312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time taken (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="378277824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -869,8 +1358,88 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Timings of</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Inverse Functions</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -885,7 +1454,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -900,7 +1469,301 @@
           <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
-    </c:legend>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$4:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>bn</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>self</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.1466666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.103333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="378280960"/>
+        <c:axId val="378278216"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="378280960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Which method</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="378278216"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="378278216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> taken for 1000 calls (seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="378280960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -976,6 +1839,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2053,20 +2956,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>114299</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2088,15 +3494,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>338137</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>300037</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>414337</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2110,6 +3516,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6417,8 +7858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N497"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10558,4 +11999,80 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1">
+        <v>0.11</v>
+      </c>
+      <c r="C1">
+        <v>0.17</v>
+      </c>
+      <c r="D1">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>5.59</v>
+      </c>
+      <c r="C2">
+        <v>15.46</v>
+      </c>
+      <c r="D2">
+        <v>15.26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <f>AVERAGE(B1:D1)</f>
+        <v>0.1466666666666667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <f>AVERAGE(B2:D2)</f>
+        <v>12.103333333333333</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>